<commit_message>
Added a power limit to OpenVehicle
This represents the rule based power limits for EVs. It is achieved by regulating the torque keeping it at the spec sheet peak torque until it is capped by the max power limit.
</commit_message>
<xml_diff>
--- a/OUR5.xlsx
+++ b/OUR5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3b07fb4c2441c8f0/Documents/GitHub/OpenLAP-Lap-Time-Simulator-EV_Mod/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="60" documentId="11_88FF5E97F77A6102EC0E57248F669B8764C9C532" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2A9FD380-CCB8-46BB-9EA0-708AA0162DEF}"/>
+  <xr:revisionPtr revIDLastSave="113" documentId="11_88FF5E97F77A6102EC0E57248F669B8764C9C532" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7815A74D-EBFD-497E-8A5C-90ADA2615B5F}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,17 +16,28 @@
     <sheet name="Info" sheetId="1" r:id="rId1"/>
     <sheet name="Torque Curve" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="91">
   <si>
     <t>General</t>
   </si>
@@ -76,9 +87,6 @@
     <t>Engine Speed [rpm]</t>
   </si>
   <si>
-    <t>Torque [Nm]</t>
-  </si>
-  <si>
     <t>Frontal Area</t>
   </si>
   <si>
@@ -290,6 +298,18 @@
   </si>
   <si>
     <t>Guestimate</t>
+  </si>
+  <si>
+    <t>Power Limit</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>Peak Torque (Nm)</t>
+  </si>
+  <si>
+    <t>Regulated Torque [Nm]</t>
   </si>
 </sst>
 </file>
@@ -353,7 +373,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -561,19 +581,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -604,11 +611,59 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -650,21 +705,29 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -676,11 +739,17 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -698,6 +767,26 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -713,11 +802,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:B26" totalsRowShown="0">
-  <autoFilter ref="A1:B26" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Engine Speed [rpm]" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Torque [Nm]"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C26" totalsRowShown="0">
+  <autoFilter ref="A1:C26" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Engine Speed [rpm]" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{189BC203-A974-43E5-A66C-A24AEFA1FDCE}" name="Peak Torque (Nm)" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Regulated Torque [Nm]" dataDxfId="0">
+      <calculatedColumnFormula>MIN(Table1[[#This Row],[Peak Torque (Nm)]],Info!$C$34*60/(2*3.1415*Table1[[#This Row],[Engine Speed '[rpm']]]))</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -986,10 +1078,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1003,40 +1095,40 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="C1" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="D1" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="E1" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="E1" s="24" t="s">
-        <v>49</v>
-      </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="36" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>86</v>
-      </c>
     </row>
     <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="33"/>
+      <c r="A3" s="37"/>
       <c r="B3" s="11" t="s">
         <v>2</v>
       </c>
@@ -1044,12 +1136,12 @@
         <v>9</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E3" s="14"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="36" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="7" t="s">
@@ -1064,7 +1156,7 @@
       <c r="E4" s="10"/>
     </row>
     <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="33"/>
+      <c r="A5" s="37"/>
       <c r="B5" s="11" t="s">
         <v>4</v>
       </c>
@@ -1075,7 +1167,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1104,74 +1196,74 @@
         <v>10</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="36" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C8" s="8">
         <v>-0.1</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="34"/>
+      <c r="A9" s="38"/>
       <c r="B9" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C9" s="3">
         <v>-1</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="34"/>
+      <c r="A10" s="38"/>
       <c r="B10" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" s="3">
         <v>1</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E10" s="20"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="34"/>
+      <c r="A11" s="38"/>
       <c r="B11" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" s="3">
         <v>1</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E11" s="20"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="34"/>
+      <c r="A12" s="38"/>
       <c r="B12" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C12" s="3">
         <v>50</v>
@@ -1182,39 +1274,39 @@
       <c r="E12" s="20"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="34"/>
+      <c r="A13" s="38"/>
       <c r="B13" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" s="3">
         <v>1.2</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E13" s="20"/>
     </row>
     <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="33"/>
+      <c r="A14" s="37"/>
       <c r="B14" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14" s="12">
         <v>1.2250000000000001</v>
       </c>
       <c r="D14" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="E14" s="14" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="32" t="s">
-        <v>20</v>
-      </c>
       <c r="B15" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15" s="8">
         <v>250</v>
@@ -1223,13 +1315,13 @@
         <v>8</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="34"/>
+      <c r="A16" s="38"/>
       <c r="B16" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C16" s="3">
         <v>40</v>
@@ -1238,43 +1330,43 @@
         <v>8</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="34"/>
+      <c r="A17" s="38"/>
       <c r="B17" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C17" s="3">
         <v>0.45</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="34"/>
+      <c r="A18" s="38"/>
       <c r="B18" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C18" s="3">
         <v>6</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="34"/>
+      <c r="A19" s="38"/>
       <c r="B19" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C19" s="3">
         <v>40</v>
@@ -1283,13 +1375,13 @@
         <v>8</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="34"/>
+      <c r="A20" s="38"/>
       <c r="B20" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C20" s="3">
         <v>25</v>
@@ -1298,88 +1390,88 @@
         <v>8</v>
       </c>
       <c r="E20" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="33"/>
+      <c r="A21" s="37"/>
       <c r="B21" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C21" s="12">
         <v>4</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="32" t="s">
+      <c r="A22" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="8">
+        <v>5</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E22" s="10"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" s="38"/>
+      <c r="B23" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C22" s="8">
-        <v>1</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E22" s="10"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="34"/>
-      <c r="B23" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C23" s="3">
+      <c r="C23" s="29">
         <v>203.2</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="34"/>
+      <c r="A24" s="38"/>
       <c r="B24" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C24" s="3">
         <v>-1E-3</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E24" s="20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="34"/>
+      <c r="A25" s="38"/>
       <c r="B25" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C25" s="3">
         <v>1.4</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E25" s="20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="34"/>
+      <c r="A26" s="38"/>
       <c r="B26" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C26" s="3">
         <v>80</v>
@@ -1388,43 +1480,43 @@
         <v>6</v>
       </c>
       <c r="E26" s="20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="34"/>
+      <c r="A27" s="38"/>
       <c r="B27" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C27" s="3">
         <v>1E-4</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" s="34"/>
+      <c r="A28" s="38"/>
       <c r="B28" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C28" s="3">
         <v>1.2</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E28" s="20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" s="34"/>
+      <c r="A29" s="38"/>
       <c r="B29" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C29" s="3">
         <v>80</v>
@@ -1433,215 +1525,228 @@
         <v>6</v>
       </c>
       <c r="E29" s="20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A30" s="34"/>
+      <c r="A30" s="38"/>
       <c r="B30" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C30" s="3">
         <v>1E-4</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E30" s="20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" s="34"/>
+      <c r="A31" s="38"/>
       <c r="B31" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C31" s="3">
         <v>800</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E31" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="33"/>
+      <c r="A32" s="39"/>
       <c r="B32" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C32" s="12">
         <v>1000</v>
       </c>
       <c r="D32" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E32" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="26" t="s">
+      <c r="A33" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="B33" s="30" t="s">
         <v>50</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>51</v>
       </c>
       <c r="C33" s="8">
         <v>1</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E33" s="10"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A34" s="29" t="s">
+    <row r="34" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="32"/>
+      <c r="B34" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="C34" s="3">
+        <v>80000</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E34" s="10"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="B35" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="C35" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C34" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E34" s="10"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A35" s="30"/>
-      <c r="B35" s="4" t="s">
+      <c r="D35" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E35" s="10"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" s="34"/>
+      <c r="B36" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C36" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="D36" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="C35" s="5">
-        <v>0.01</v>
-      </c>
-      <c r="D35" s="6" t="s">
+      <c r="E36" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="E35" s="25" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A36" s="30"/>
-      <c r="B36" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C36" s="5">
-        <v>1</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E36" s="25" t="s">
-        <v>81</v>
-      </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A37" s="30"/>
+      <c r="A37" s="34"/>
       <c r="B37" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C37" s="5">
         <v>1</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E37" s="25" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" s="30"/>
+      <c r="A38" s="34"/>
       <c r="B38" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C38" s="5">
-        <v>0.92</v>
+        <v>1</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E38" s="25" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A39" s="30"/>
-      <c r="B39" s="1" t="s">
+      <c r="A39" s="34"/>
+      <c r="B39" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C39" s="5">
+        <v>0.92</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E39" s="25" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A40" s="34"/>
+      <c r="B40" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C40" s="3">
+        <v>1</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E40" s="20" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A41" s="34"/>
+      <c r="B41" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C39" s="3">
+      <c r="C41" s="3">
+        <v>4.2</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E41" s="20"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A42" s="34"/>
+      <c r="B42" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="C42" s="3">
         <v>1</v>
       </c>
-      <c r="D39" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E39" s="20" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" s="30"/>
-      <c r="B40" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C40" s="3">
-        <v>4.2</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E40" s="20"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41" s="30"/>
-      <c r="B41" s="27" t="s">
-        <v>84</v>
-      </c>
-      <c r="C41" s="3">
-        <v>1</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E41" s="20"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A42" s="30"/>
+      <c r="D42" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E42" s="20"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A43" s="30"/>
+      <c r="A43" s="34"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A44" s="30"/>
+      <c r="A44" s="34"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45" s="30"/>
+      <c r="A45" s="34"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A46" s="30"/>
+      <c r="A46" s="34"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47" s="30"/>
+      <c r="A47" s="34"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A48" s="30"/>
+      <c r="A48" s="34"/>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A49" s="30"/>
-    </row>
-    <row r="50" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="31"/>
+      <c r="A49" s="34"/>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A50" s="34"/>
+    </row>
+    <row r="51" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A51" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A34:A50"/>
+    <mergeCell ref="A35:A51"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="A8:A14"/>
@@ -1655,224 +1760,328 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="21.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="28">
+        <v>89</v>
+      </c>
+      <c r="C1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="27">
         <v>1</v>
       </c>
       <c r="B2">
         <v>254.56049999999999</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="28">
+      <c r="C2" s="28">
+        <f>MIN(Table1[[#This Row],[Peak Torque (Nm)]],Info!$C$34*60/(2*3.1415*Table1[[#This Row],[Engine Speed '[rpm']]]))</f>
+        <v>254.56049999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="27">
         <v>250</v>
       </c>
       <c r="B3">
         <v>254.56809999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="28">
+      <c r="C3" s="28">
+        <f>MIN(Table1[[#This Row],[Peak Torque (Nm)]],Info!$C$34*60/(2*3.1415*Table1[[#This Row],[Engine Speed '[rpm']]]))</f>
+        <v>254.56809999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="27">
         <v>500</v>
       </c>
       <c r="B4">
         <v>254.55430000000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="28">
+      <c r="C4" s="28">
+        <f>MIN(Table1[[#This Row],[Peak Torque (Nm)]],Info!$C$34*60/(2*3.1415*Table1[[#This Row],[Engine Speed '[rpm']]]))</f>
+        <v>254.55430000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="27">
         <v>750</v>
       </c>
       <c r="B5">
         <v>254.5334</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="28">
+      <c r="C5" s="28">
+        <f>MIN(Table1[[#This Row],[Peak Torque (Nm)]],Info!$C$34*60/(2*3.1415*Table1[[#This Row],[Engine Speed '[rpm']]]))</f>
+        <v>254.5334</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="27">
         <v>1000</v>
       </c>
       <c r="B6">
         <v>254.50839999999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="28">
+      <c r="C6" s="28">
+        <f>MIN(Table1[[#This Row],[Peak Torque (Nm)]],Info!$C$34*60/(2*3.1415*Table1[[#This Row],[Engine Speed '[rpm']]]))</f>
+        <v>254.50839999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="27">
         <v>1250</v>
       </c>
       <c r="B7">
         <v>254.48</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="28">
+      <c r="C7" s="28">
+        <f>MIN(Table1[[#This Row],[Peak Torque (Nm)]],Info!$C$34*60/(2*3.1415*Table1[[#This Row],[Engine Speed '[rpm']]]))</f>
+        <v>254.48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="27">
         <v>1500</v>
       </c>
       <c r="B8">
         <v>254.44880000000001</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="28">
+      <c r="C8" s="28">
+        <f>MIN(Table1[[#This Row],[Peak Torque (Nm)]],Info!$C$34*60/(2*3.1415*Table1[[#This Row],[Engine Speed '[rpm']]]))</f>
+        <v>254.44880000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="27">
         <v>1750</v>
       </c>
       <c r="B9">
         <v>254.41499999999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" s="28">
+      <c r="C9" s="28">
+        <f>MIN(Table1[[#This Row],[Peak Torque (Nm)]],Info!$C$34*60/(2*3.1415*Table1[[#This Row],[Engine Speed '[rpm']]]))</f>
+        <v>254.41499999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="27">
         <v>2000</v>
       </c>
       <c r="B10">
         <v>254.3785</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" s="28">
+      <c r="C10" s="28">
+        <f>MIN(Table1[[#This Row],[Peak Torque (Nm)]],Info!$C$34*60/(2*3.1415*Table1[[#This Row],[Engine Speed '[rpm']]]))</f>
+        <v>254.3785</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="27">
         <v>2250</v>
       </c>
       <c r="B11">
         <v>254.33969999999999</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" s="28">
+      <c r="C11" s="28">
+        <f>MIN(Table1[[#This Row],[Peak Torque (Nm)]],Info!$C$34*60/(2*3.1415*Table1[[#This Row],[Engine Speed '[rpm']]]))</f>
+        <v>254.33969999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="27">
         <v>2500</v>
       </c>
       <c r="B12">
         <v>254.29830000000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" s="28">
+      <c r="C12" s="28">
+        <f>MIN(Table1[[#This Row],[Peak Torque (Nm)]],Info!$C$34*60/(2*3.1415*Table1[[#This Row],[Engine Speed '[rpm']]]))</f>
+        <v>254.29830000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" s="27">
         <v>2750</v>
       </c>
       <c r="B13">
         <v>254.25460000000001</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" s="28">
+      <c r="C13" s="28">
+        <f>MIN(Table1[[#This Row],[Peak Torque (Nm)]],Info!$C$34*60/(2*3.1415*Table1[[#This Row],[Engine Speed '[rpm']]]))</f>
+        <v>254.25460000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" s="27">
         <v>3000</v>
       </c>
       <c r="B14">
         <v>254.20849999999999</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" s="28">
+      <c r="C14" s="28">
+        <f>MIN(Table1[[#This Row],[Peak Torque (Nm)]],Info!$C$34*60/(2*3.1415*Table1[[#This Row],[Engine Speed '[rpm']]]))</f>
+        <v>254.20849999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" s="27">
         <v>3250</v>
       </c>
       <c r="B15">
         <v>254.1601</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" s="28">
+      <c r="C15" s="28">
+        <f>MIN(Table1[[#This Row],[Peak Torque (Nm)]],Info!$C$34*60/(2*3.1415*Table1[[#This Row],[Engine Speed '[rpm']]]))</f>
+        <v>235.06654097136351</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" s="27">
         <v>3500</v>
       </c>
       <c r="B16">
         <v>254.10929999999999</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" s="28">
+      <c r="C16" s="28">
+        <f>MIN(Table1[[#This Row],[Peak Torque (Nm)]],Info!$C$34*60/(2*3.1415*Table1[[#This Row],[Engine Speed '[rpm']]]))</f>
+        <v>218.27607375912325</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="27">
         <v>3750</v>
       </c>
       <c r="B17">
         <v>254.05619999999999</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" s="28">
+      <c r="C17" s="28">
+        <f>MIN(Table1[[#This Row],[Peak Torque (Nm)]],Info!$C$34*60/(2*3.1415*Table1[[#This Row],[Engine Speed '[rpm']]]))</f>
+        <v>203.72433550851505</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" s="27">
         <v>4000</v>
       </c>
       <c r="B18">
         <v>253.96430000000001</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" s="28">
+      <c r="C18" s="28">
+        <f>MIN(Table1[[#This Row],[Peak Torque (Nm)]],Info!$C$34*60/(2*3.1415*Table1[[#This Row],[Engine Speed '[rpm']]]))</f>
+        <v>190.99156453923285</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="27">
         <v>4250</v>
       </c>
       <c r="B19">
         <v>250.97919999999999</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" s="28">
+      <c r="C19" s="28">
+        <f>MIN(Table1[[#This Row],[Peak Torque (Nm)]],Info!$C$34*60/(2*3.1415*Table1[[#This Row],[Engine Speed '[rpm']]]))</f>
+        <v>179.75676662516034</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="27">
         <v>4500</v>
       </c>
       <c r="B20">
         <v>244.5763</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" s="28">
+      <c r="C20" s="28">
+        <f>MIN(Table1[[#This Row],[Peak Torque (Nm)]],Info!$C$34*60/(2*3.1415*Table1[[#This Row],[Engine Speed '[rpm']]]))</f>
+        <v>169.7702795904292</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="27">
         <v>4750</v>
       </c>
       <c r="B21">
         <v>236.43809999999999</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" s="28">
+      <c r="C21" s="28">
+        <f>MIN(Table1[[#This Row],[Peak Torque (Nm)]],Info!$C$34*60/(2*3.1415*Table1[[#This Row],[Engine Speed '[rpm']]]))</f>
+        <v>160.83500171724873</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" s="27">
         <v>5000</v>
       </c>
       <c r="B22">
         <v>227.55119999999999</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23" s="28">
+      <c r="C22" s="28">
+        <f>MIN(Table1[[#This Row],[Peak Torque (Nm)]],Info!$C$34*60/(2*3.1415*Table1[[#This Row],[Engine Speed '[rpm']]]))</f>
+        <v>152.79325163138628</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" s="27">
         <v>5250</v>
       </c>
       <c r="B23">
         <v>218.0162</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" s="28">
+      <c r="C23" s="28">
+        <f>MIN(Table1[[#This Row],[Peak Torque (Nm)]],Info!$C$34*60/(2*3.1415*Table1[[#This Row],[Engine Speed '[rpm']]]))</f>
+        <v>145.51738250608219</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" s="27">
         <v>5500</v>
       </c>
       <c r="B24">
         <v>208.19040000000001</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" s="28">
+      <c r="C24" s="28">
+        <f>MIN(Table1[[#This Row],[Peak Torque (Nm)]],Info!$C$34*60/(2*3.1415*Table1[[#This Row],[Engine Speed '[rpm']]]))</f>
+        <v>138.90295602853297</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" s="27">
         <v>5750</v>
       </c>
       <c r="B25">
         <v>198</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26" s="28">
+      <c r="C25" s="28">
+        <f>MIN(Table1[[#This Row],[Peak Torque (Nm)]],Info!$C$34*60/(2*3.1415*Table1[[#This Row],[Engine Speed '[rpm']]]))</f>
+        <v>132.86369707077068</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" s="27">
         <v>6000</v>
       </c>
       <c r="B26">
         <v>189</v>
+      </c>
+      <c r="C26" s="28">
+        <f>MIN(Table1[[#This Row],[Peak Torque (Nm)]],Info!$C$34*60/(2*3.1415*Table1[[#This Row],[Engine Speed '[rpm']]]))</f>
+        <v>127.3277096928219</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed gearing from OpenDrag
Removed gearing from opendrag and fixed the average decelaration to consider non-stopped cars. Lastly, switched acceleration to match event.
</commit_message>
<xml_diff>
--- a/OUR5.xlsx
+++ b/OUR5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3b07fb4c2441c8f0/Documents/GitHub/OpenLAP-Lap-Time-Simulator-EV_Mod/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="178" documentId="11_88FF5E97F77A6102EC0E57248F669B8764C9C532" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{46670C61-A07C-4BC6-9350-1870B34BBAFC}"/>
+  <xr:revisionPtr revIDLastSave="180" documentId="11_88FF5E97F77A6102EC0E57248F669B8764C9C532" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{83489F43-6A02-4EC0-8896-61E14AF35901}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="93">
   <si>
     <t>General</t>
   </si>
@@ -1129,7 +1129,7 @@
   <dimension ref="A1:E52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1655,7 +1655,7 @@
         <v>87</v>
       </c>
       <c r="C35" s="3">
-        <v>60000</v>
+        <v>80000</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>88</v>
@@ -1697,8 +1697,8 @@
       <c r="B38" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C38" s="5">
-        <v>1</v>
+      <c r="C38" s="5" t="s">
+        <v>66</v>
       </c>
       <c r="D38" s="6" t="s">
         <v>37</v>
@@ -1824,7 +1824,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B26"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2008,7 +2008,7 @@
       </c>
       <c r="C12" s="26">
         <f>MIN(Table1[[#This Row],[Peak Torque (Nm)]],Info!$C$35*60/(2*3.1415*Table1[[#This Row],[Engine Speed '[rpm']]]))</f>
-        <v>229.18987744707943</v>
+        <v>254.29830000000001</v>
       </c>
       <c r="D12">
         <v>0.95</v>
@@ -2023,7 +2023,7 @@
       </c>
       <c r="C13" s="26">
         <f>MIN(Table1[[#This Row],[Peak Torque (Nm)]],Info!$C$35*60/(2*3.1415*Table1[[#This Row],[Engine Speed '[rpm']]]))</f>
-        <v>208.35443404279948</v>
+        <v>254.25460000000001</v>
       </c>
       <c r="D13">
         <v>0.95</v>
@@ -2038,7 +2038,7 @@
       </c>
       <c r="C14" s="26">
         <f>MIN(Table1[[#This Row],[Peak Torque (Nm)]],Info!$C$35*60/(2*3.1415*Table1[[#This Row],[Engine Speed '[rpm']]]))</f>
-        <v>190.99156453923285</v>
+        <v>253.98330000000001</v>
       </c>
       <c r="D14">
         <v>0.95</v>
@@ -2053,7 +2053,7 @@
       </c>
       <c r="C15" s="26">
         <f>MIN(Table1[[#This Row],[Peak Torque (Nm)]],Info!$C$35*60/(2*3.1415*Table1[[#This Row],[Engine Speed '[rpm']]]))</f>
-        <v>176.29990572852262</v>
+        <v>235.06654097136351</v>
       </c>
       <c r="D15">
         <v>0.95</v>
@@ -2068,7 +2068,7 @@
       </c>
       <c r="C16" s="26">
         <f>MIN(Table1[[#This Row],[Peak Torque (Nm)]],Info!$C$35*60/(2*3.1415*Table1[[#This Row],[Engine Speed '[rpm']]]))</f>
-        <v>163.70705531934243</v>
+        <v>218.27607375912325</v>
       </c>
       <c r="D16">
         <v>0.95</v>
@@ -2083,7 +2083,7 @@
       </c>
       <c r="C17" s="26">
         <f>MIN(Table1[[#This Row],[Peak Torque (Nm)]],Info!$C$35*60/(2*3.1415*Table1[[#This Row],[Engine Speed '[rpm']]]))</f>
-        <v>152.79325163138628</v>
+        <v>203.72433550851505</v>
       </c>
       <c r="D17">
         <v>0.95</v>
@@ -2098,7 +2098,7 @@
       </c>
       <c r="C18" s="26">
         <f>MIN(Table1[[#This Row],[Peak Torque (Nm)]],Info!$C$35*60/(2*3.1415*Table1[[#This Row],[Engine Speed '[rpm']]]))</f>
-        <v>143.24367340442464</v>
+        <v>190.99156453923285</v>
       </c>
       <c r="D18">
         <v>0.95</v>
@@ -2113,7 +2113,7 @@
       </c>
       <c r="C19" s="26">
         <f>MIN(Table1[[#This Row],[Peak Torque (Nm)]],Info!$C$35*60/(2*3.1415*Table1[[#This Row],[Engine Speed '[rpm']]]))</f>
-        <v>134.81757496887025</v>
+        <v>179.75676662516034</v>
       </c>
       <c r="D19">
         <v>0.95</v>
@@ -2128,7 +2128,7 @@
       </c>
       <c r="C20" s="26">
         <f>MIN(Table1[[#This Row],[Peak Torque (Nm)]],Info!$C$35*60/(2*3.1415*Table1[[#This Row],[Engine Speed '[rpm']]]))</f>
-        <v>127.3277096928219</v>
+        <v>169.7702795904292</v>
       </c>
       <c r="D20">
         <v>0.9</v>
@@ -2143,7 +2143,7 @@
       </c>
       <c r="C21" s="26">
         <f>MIN(Table1[[#This Row],[Peak Torque (Nm)]],Info!$C$35*60/(2*3.1415*Table1[[#This Row],[Engine Speed '[rpm']]]))</f>
-        <v>120.62625128793654</v>
+        <v>160.83500171724873</v>
       </c>
       <c r="D21">
         <v>0.88</v>
@@ -2158,7 +2158,7 @@
       </c>
       <c r="C22" s="26">
         <f>MIN(Table1[[#This Row],[Peak Torque (Nm)]],Info!$C$35*60/(2*3.1415*Table1[[#This Row],[Engine Speed '[rpm']]]))</f>
-        <v>114.59493872353971</v>
+        <v>152.79325163138628</v>
       </c>
       <c r="D22">
         <v>0.84</v>
@@ -2173,7 +2173,7 @@
       </c>
       <c r="C23" s="26">
         <f>MIN(Table1[[#This Row],[Peak Torque (Nm)]],Info!$C$35*60/(2*3.1415*Table1[[#This Row],[Engine Speed '[rpm']]]))</f>
-        <v>109.13803687956162</v>
+        <v>145.51738250608219</v>
       </c>
       <c r="D23">
         <v>0.81</v>
@@ -2188,7 +2188,7 @@
       </c>
       <c r="C24" s="26">
         <f>MIN(Table1[[#This Row],[Peak Torque (Nm)]],Info!$C$35*60/(2*3.1415*Table1[[#This Row],[Engine Speed '[rpm']]]))</f>
-        <v>104.17721702139974</v>
+        <v>138.90295602853297</v>
       </c>
       <c r="D24">
         <v>0.79</v>
@@ -2203,7 +2203,7 @@
       </c>
       <c r="C25" s="26">
         <f>MIN(Table1[[#This Row],[Peak Torque (Nm)]],Info!$C$35*60/(2*3.1415*Table1[[#This Row],[Engine Speed '[rpm']]]))</f>
-        <v>99.647772803078013</v>
+        <v>132.86369707077068</v>
       </c>
       <c r="D25">
         <v>0.77</v>
@@ -2218,7 +2218,7 @@
       </c>
       <c r="C26" s="26">
         <f>MIN(Table1[[#This Row],[Peak Torque (Nm)]],Info!$C$35*60/(2*3.1415*Table1[[#This Row],[Engine Speed '[rpm']]]))</f>
-        <v>95.495782269616427</v>
+        <v>127.3277096928219</v>
       </c>
       <c r="D26">
         <v>0.75</v>

</xml_diff>